<commit_message>
other fields and interest income expence logic home 6 July 2023
</commit_message>
<xml_diff>
--- a/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/notes_transformed_standard_cropped_df.xlsx
+++ b/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/notes_transformed_standard_cropped_df.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="122">
   <si>
     <t>rows</t>
   </si>
@@ -51,25 +51,25 @@
     <t>value</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cash at bank and on hand</t>
+    <t>None Cash at bank and on hand</t>
   </si>
   <si>
     <t>$000</t>
   </si>
   <si>
-    <t xml:space="preserve"> GST receivable</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Related party receivables (Note 20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Raw materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Finished goods</t>
+    <t>None GST receivable</t>
+  </si>
+  <si>
+    <t>None Related party receivables (Note 20)</t>
+  </si>
+  <si>
+    <t>None Total</t>
+  </si>
+  <si>
+    <t>None Raw materials</t>
+  </si>
+  <si>
+    <t>None Finished goods</t>
   </si>
   <si>
     <t>Current Foreign exchange derivatives at fair value</t>
@@ -78,7 +78,7 @@
     <t>Current Electricity derivatives at fair value</t>
   </si>
   <si>
-    <t xml:space="preserve">Current </t>
+    <t>Current Total</t>
   </si>
   <si>
     <t>Non-current Electricity derivatives at fair value</t>
@@ -93,19 +93,19 @@
     <t>Ownership interest $000</t>
   </si>
   <si>
-    <t xml:space="preserve"> At 1 January</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Share of gain/(loss) of joint venture, net of tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Share of other comprehensive income, net of tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Carrying value of investment at end of year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Investment in joint venture (Southern Cross Aluminium Pty Ltd)</t>
+    <t>None At 1 January</t>
+  </si>
+  <si>
+    <t>None Share of gain/(loss) of joint venture, net of tax</t>
+  </si>
+  <si>
+    <t>None Share of other comprehensive income, net of tax</t>
+  </si>
+  <si>
+    <t>None Carrying value of investment at end of year</t>
+  </si>
+  <si>
+    <t>None Investment in joint venture (Southern Cross Aluminium Pty Ltd)</t>
   </si>
   <si>
     <t>Cost At 1 January 2020</t>
@@ -171,70 +171,70 @@
     <t>Income tax benefit reported in the statement of profit or loss and other comprehensive income</t>
   </si>
   <si>
-    <t xml:space="preserve"> Accounting loss before income tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> At Australia's statutory income tax rate of 30% (2019: 30%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amounts not deductible for tax purposes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Adjustments in respect of current income tax of previous year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Income tax benefit reported in profit or loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As of 1 January</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Income tax benefit during the year recognised in profit or loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Income tax benefit during the year recognised in other comprehensive income</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> As at 31 December</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trade and other receivables</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Financial assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Property, plant and equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Right-of-use assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trade and other payables</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Provisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lease liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Financial liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ARO assets</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Deferred tax benefit</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Net deferred tax assets/liabilities)</t>
+    <t>None Accounting loss before income tax</t>
+  </si>
+  <si>
+    <t>None At Australia's statutory income tax rate of 30% (2019: 30%)</t>
+  </si>
+  <si>
+    <t>None Amounts not deductible for tax purposes</t>
+  </si>
+  <si>
+    <t>None Adjustments in respect of current income tax of previous year</t>
+  </si>
+  <si>
+    <t>None Others</t>
+  </si>
+  <si>
+    <t>None Income tax benefit reported in profit or loss</t>
+  </si>
+  <si>
+    <t>None As of 1 January</t>
+  </si>
+  <si>
+    <t>None Income tax benefit during the year recognised in profit or loss</t>
+  </si>
+  <si>
+    <t>None Income tax benefit during the year recognised in other comprehensive income</t>
+  </si>
+  <si>
+    <t>None As at 31 December</t>
+  </si>
+  <si>
+    <t>None Trade and other receivables</t>
+  </si>
+  <si>
+    <t>None Financial assets</t>
+  </si>
+  <si>
+    <t>None Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>None Right-of-use assets</t>
+  </si>
+  <si>
+    <t>None Other assets</t>
+  </si>
+  <si>
+    <t>None Trade and other payables</t>
+  </si>
+  <si>
+    <t>None Provisions</t>
+  </si>
+  <si>
+    <t>None Lease liabilities</t>
+  </si>
+  <si>
+    <t>None Financial liabilities</t>
+  </si>
+  <si>
+    <t>None ARO assets</t>
+  </si>
+  <si>
+    <t>None Deferred tax benefit</t>
+  </si>
+  <si>
+    <t>None Net deferred tax assets/liabilities)</t>
   </si>
   <si>
     <t>as follows: Deferred tax assets</t>
@@ -249,19 +249,19 @@
     <t>Statement of profit or loss Statement of financial and other comprehensive position income $000</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bank borrowings</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> facilities facilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Utilised </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Utilised bank guarantees</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Balance at 31 December Balance at 31 December</t>
+    <t>None Bank borrowings</t>
+  </si>
+  <si>
+    <t>None facilities facilities</t>
+  </si>
+  <si>
+    <t>None Utilised nan</t>
+  </si>
+  <si>
+    <t>None Utilised bank guarantees</t>
+  </si>
+  <si>
+    <t>None Balance at 31 December Balance at 31 December</t>
   </si>
   <si>
     <t>Multi-option facilities $000</t>
@@ -270,22 +270,22 @@
     <t>Bank guarantee facilities $000</t>
   </si>
   <si>
-    <t xml:space="preserve"> At 1 January 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arising during the year</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Unwinding of discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> At31 December 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Non-current</t>
+    <t>None At 1 January 2020</t>
+  </si>
+  <si>
+    <t>None Arising during the year</t>
+  </si>
+  <si>
+    <t>None Unwinding of discount</t>
+  </si>
+  <si>
+    <t>None At31 December 2020</t>
+  </si>
+  <si>
+    <t>None 2020 Current</t>
+  </si>
+  <si>
+    <t>None 2020 Non-current</t>
   </si>
   <si>
     <t>Employee benefits</t>
@@ -306,10 +306,16 @@
     <t>Totals</t>
   </si>
   <si>
-    <t xml:space="preserve"> Electricity derivatives at fair value through OCI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 155,299,534 ordinary shares issued and fully paid (2019: 155,299,534)</t>
+    <t>None Electricity derivatives at fair value through OCI</t>
+  </si>
+  <si>
+    <t>None Current</t>
+  </si>
+  <si>
+    <t>None Non-current</t>
+  </si>
+  <si>
+    <t>None 155,299,534 ordinary shares issued and fully paid (2019: 155,299,534)</t>
   </si>
   <si>
     <t>Cash flow hedge reserve Balance at 1 January</t>
@@ -321,7 +327,7 @@
     <t>Cash flow hedge reserve Balance at 31 December</t>
   </si>
   <si>
-    <t xml:space="preserve">Cash flow hedge reserve </t>
+    <t>Cash flow hedge reserve Total</t>
   </si>
   <si>
     <t>Reserve in joint venture Balance at 1 January</t>
@@ -333,7 +339,7 @@
     <t>Reserve in joint venture Balance at 31 December</t>
   </si>
   <si>
-    <t xml:space="preserve">Reserve in joint venture </t>
+    <t>Reserve in joint venture Total</t>
   </si>
   <si>
     <t>Other reserve Balance at 1 January</t>
@@ -342,7 +348,7 @@
     <t>Other reserve Balance at 31 December</t>
   </si>
   <si>
-    <t xml:space="preserve">Other reserve </t>
+    <t>Other reserve Total</t>
   </si>
   <si>
     <t>Total Balance at 1 January</t>
@@ -375,28 +381,28 @@
     <t>Timing of revenue recognition Total revenue from contracts with customers</t>
   </si>
   <si>
-    <t xml:space="preserve"> Commission revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Government grants</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Insurance proceeds</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Foreign exchange gain</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bank interest</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Interest expenses</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Discount unwind on the provision for asset retirement obligation</t>
+    <t>None Commission revenue</t>
+  </si>
+  <si>
+    <t>None Government grants</t>
+  </si>
+  <si>
+    <t>None Insurance proceeds</t>
+  </si>
+  <si>
+    <t>None Foreign exchange gain</t>
+  </si>
+  <si>
+    <t>None Other</t>
+  </si>
+  <si>
+    <t>None Bank interest</t>
+  </si>
+  <si>
+    <t>None Interest expenses</t>
+  </si>
+  <si>
+    <t>None Discount unwind on the provision for asset retirement obligation</t>
   </si>
 </sst>
 </file>
@@ -3120,7 +3126,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -3134,7 +3140,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -3175,7 +3181,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -3189,7 +3195,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3230,7 +3236,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -3244,7 +3250,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3258,7 +3264,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -3272,7 +3278,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -3286,7 +3292,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -3300,7 +3306,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -3314,7 +3320,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -3328,7 +3334,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -3342,7 +3348,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -3356,7 +3362,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -3370,7 +3376,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -3384,7 +3390,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -3398,7 +3404,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -3412,7 +3418,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -3440,7 +3446,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -3468,7 +3474,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -3482,7 +3488,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -3496,7 +3502,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -3510,7 +3516,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -3524,7 +3530,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3538,7 +3544,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -3552,7 +3558,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -3566,7 +3572,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3580,7 +3586,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -3594,7 +3600,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -3608,7 +3614,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -3622,7 +3628,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -3636,7 +3642,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -3650,7 +3656,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -3664,7 +3670,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -3678,7 +3684,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -3692,7 +3698,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -3844,7 +3850,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -3858,7 +3864,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3872,7 +3878,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -3886,7 +3892,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -3900,7 +3906,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -3914,7 +3920,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -3928,7 +3934,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -3942,7 +3948,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -3956,7 +3962,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -3970,7 +3976,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -3984,7 +3990,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -3998,7 +4004,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -4012,7 +4018,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -4026,7 +4032,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -4067,7 +4073,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -4081,7 +4087,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -4122,7 +4128,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -4136,7 +4142,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -4150,7 +4156,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -4164,7 +4170,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -4192,7 +4198,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -4206,7 +4212,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -4220,7 +4226,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -4234,7 +4240,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -4289,7 +4295,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -4303,7 +4309,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -4344,7 +4350,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -4358,7 +4364,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -4386,7 +4392,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -4400,7 +4406,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>

</xml_diff>